<commit_message>
pc change binary 1013
</commit_message>
<xml_diff>
--- a/binaryFile.xlsx
+++ b/binaryFile.xlsx
@@ -16,9 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>blah</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc changes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -376,6 +380,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PC changes again 1028
</commit_message>
<xml_diff>
--- a/binaryFile.xlsx
+++ b/binaryFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>blah</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Laptop changes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC changes again</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,22 +373,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -400,7 +409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -413,7 +422,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pc refuses any changes 1020
</commit_message>
<xml_diff>
--- a/binaryFile.xlsx
+++ b/binaryFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>blah</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -27,6 +27,10 @@
   </si>
   <si>
     <t>PC changes again</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC refuses any changes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -373,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -396,6 +400,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>